<commit_message>
ci(Update): Add new SQL tables to database model
This commit introduces multiple new SQL tables to the MyExpenses
database model. The tables include `t_account_type`, `t_account`,
`t_category_type`,  `t_mode_payment`, `t_place`, and `t_history`. Each
of these tables contributes to a more detailed and voracious data
structure for financial tracking transactions.
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZP6177\Creative Cloud Files\Programmation\C#\Personnel\MyExpenses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZP6177\Creative Cloud Files\Programmation\C#\Ineo Infracom\MyExpenses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF958B5-0EBE-4229-879F-0ECBC0FDD75A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACAAB49-13AC-44DB-9272-E8D74B2BB454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{3C8728D4-4D3D-4C35-A3FE-37BAB581B7CE}"/>
+    <workbookView xWindow="22932" yWindow="-168" windowWidth="30936" windowHeight="18816" xr2:uid="{3C8728D4-4D3D-4C35-A3FE-37BAB581B7CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -374,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -412,6 +412,21 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -436,22 +451,13 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -462,9 +468,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF0066"/>
       <color rgb="FF6666FF"/>
       <color rgb="FFABF1BC"/>
-      <color rgb="FFFF0066"/>
       <color rgb="FFFF00FF"/>
     </mruColors>
   </colors>
@@ -776,48 +782,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{308B6434-A4D7-4BAC-9CEC-2A04A709C66A}">
-  <dimension ref="B2:W24"/>
+  <dimension ref="B2:W20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="12" max="12" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B2" s="13" t="s">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
       <c r="L2" s="9"/>
-      <c r="N2" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
-      <c r="V2" s="24"/>
-      <c r="W2" s="24"/>
-    </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -842,51 +852,21 @@
       <c r="I3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="P3" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="W3" s="26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="10" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -907,60 +887,68 @@
       <c r="I4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K4" s="6" t="s">
+      <c r="N4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="O4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="N6" s="16" t="s">
+      <c r="P4" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B6" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="G6" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="14"/>
+      <c r="J6" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="16"/>
+      <c r="N6" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="16"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="16"/>
-      <c r="V6" s="16"/>
-    </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="27"/>
+      <c r="T6" s="27"/>
+      <c r="U6" s="27"/>
+      <c r="V6" s="28"/>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="N7" s="1" t="s">
         <v>0</v>
       </c>
@@ -989,7 +977,31 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1018,33 +1030,35 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="N10" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20"/>
-      <c r="S10" s="17" t="s">
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B10" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="N10" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="O10" s="19"/>
+      <c r="S10" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="T10" s="18"/>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="19"/>
-    </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="T10" s="23"/>
+      <c r="U10" s="23"/>
+      <c r="V10" s="23"/>
+      <c r="W10" s="24"/>
+    </row>
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="N11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P11" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="S11" s="1" t="s">
         <v>0</v>
@@ -1062,19 +1076,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P12" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="S12" s="1" t="s">
         <v>4</v>
       </c>
@@ -1089,182 +1103,184 @@
       </c>
       <c r="W12" s="1"/>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="N14" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="O14" s="22"/>
-      <c r="Q14" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="R14" s="14"/>
-      <c r="T14" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="U14" s="15"/>
-    </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B14" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="N14" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="O14" s="15"/>
+    </row>
+    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="N15" s="1" t="s">
         <v>0</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="Q15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="U15" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="N16" s="1" t="s">
         <v>4</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Q16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="T16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U16" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="14:22" x14ac:dyDescent="0.3">
-      <c r="N18" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="O18" s="23"/>
-      <c r="Q18" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="R18" s="25"/>
-    </row>
-    <row r="19" spans="14:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="14:22" x14ac:dyDescent="0.25">
+      <c r="N18" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13"/>
+      <c r="V18" s="13"/>
+    </row>
+    <row r="19" spans="14:22" x14ac:dyDescent="0.25">
       <c r="N19" s="1" t="s">
         <v>0</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="14:22" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="S19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V19" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="14:22" x14ac:dyDescent="0.25">
       <c r="N20" s="1" t="s">
         <v>4</v>
       </c>
       <c r="O20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="14:22" x14ac:dyDescent="0.3">
-      <c r="N22" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="O22" s="21"/>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="21"/>
-      <c r="S22" s="21"/>
-      <c r="T22" s="21"/>
-      <c r="U22" s="21"/>
-      <c r="V22" s="21"/>
-    </row>
-    <row r="23" spans="14:22" x14ac:dyDescent="0.3">
-      <c r="N23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q23" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="R23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="S23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="T23" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="U23" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="V23" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="14:22" x14ac:dyDescent="0.3">
-      <c r="N24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="O24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q24" s="1" t="s">
+      <c r="S20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="R24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S24" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="T24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="V24" s="4" t="s">
+      <c r="V20" s="4" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="N22:V22"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="S10:W10"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="N6:V6"/>
+    <mergeCell ref="N18:V18"/>
+    <mergeCell ref="G6:H6"/>
     <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="N2:W2"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="T14:U14"/>
-    <mergeCell ref="N6:V6"/>
-    <mergeCell ref="S10:W10"/>
-    <mergeCell ref="N10:Q10"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B14:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1279,37 +1295,37 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="14" max="14" width="12.33203125" customWidth="1"/>
-    <col min="16" max="16" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" customWidth="1"/>
+    <col min="16" max="16" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B2" s="13" t="s">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="L2" s="24" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="L2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-    </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1365,7 +1381,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -1421,7 +1437,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -1450,18 +1466,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="L6" s="16" t="s">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="L6" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-    </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="21"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="L7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1484,7 +1500,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="L8" s="1">
         <v>1</v>
       </c>
@@ -1507,17 +1523,17 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="L10" s="23" t="s">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="L10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="M10" s="23"/>
-      <c r="O10" s="25" t="s">
+      <c r="M10" s="15"/>
+      <c r="O10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="P10" s="25"/>
-    </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="P10" s="16"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="L11" s="1">
         <v>1</v>
       </c>
@@ -1531,7 +1547,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="L12" s="1">
         <v>2</v>
       </c>
@@ -1545,17 +1561,17 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="L14" s="22" t="s">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="L14" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="M14" s="22"/>
-      <c r="O14" s="14" t="s">
+      <c r="M14" s="14"/>
+      <c r="O14" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="P14" s="14"/>
-    </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="P14" s="19"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="L15" s="1" t="s">
         <v>0</v>
       </c>
@@ -1569,7 +1585,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="L16" s="1">
         <v>1</v>
       </c>

</xml_diff>